<commit_message>
Added Mixed ANOVA Tests
Added the Mixed ANOVA tests and the related assumption checks. I need to make more graphs and actually export them, but that'll come later.
</commit_message>
<xml_diff>
--- a/imports/vpl-fnl_pjt_data.xlsx
+++ b/imports/vpl-fnl_pjt_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roder\source\year 4 repos\HCI-FNL_PJT\imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7196A7A6-AD61-4B1A-BC3B-B1F0F13A2060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45C2502-05EA-4CBC-81EA-D49BE157EF54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{648EF0DD-0358-465E-A7D1-701403DC3CB5}"/>
   </bookViews>
@@ -34,24 +34,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>Participant</t>
   </si>
   <si>
-    <t>TBD01</t>
-  </si>
-  <si>
-    <t>TBD02</t>
-  </si>
-  <si>
-    <t>TBD03</t>
-  </si>
-  <si>
-    <t>TBD04</t>
-  </si>
-  <si>
-    <t>TBDB05</t>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>A-&gt;B</t>
+  </si>
+  <si>
+    <t>B-&gt;A</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Kills</t>
+  </si>
+  <si>
+    <t>Hit_Percent</t>
+  </si>
+  <si>
+    <t>Shots_Hit</t>
+  </si>
+  <si>
+    <t>Shots_Fired</t>
   </si>
 </sst>
 </file>
@@ -403,18 +421,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73DA4086-D66D-4A32-8F38-A033B2F7B296}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,146 +443,268 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="B2">
-        <f>1</f>
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <f>1</f>
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
       <c r="D2">
-        <f>1</f>
-        <v>1</v>
+        <v>10.5</v>
       </c>
       <c r="E2">
         <f>1</f>
         <v>1</v>
       </c>
       <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2">
         <f>1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H2">
+        <f>G2/F2*100</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f>A2+1</f>
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <f t="shared" ref="B3:F6" si="0">B2+1</f>
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" ref="D3:G5" si="0">D2+1</f>
+        <v>11.5</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F3">
+        <v>15</v>
+      </c>
+      <c r="G3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <f t="shared" ref="H3:H4" si="1">G3/F3*100</f>
+        <v>13.333333333333334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f t="shared" ref="A4:A6" si="1">A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>12.5</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="F4">
+        <f>19</f>
+        <v>19</v>
+      </c>
+      <c r="G4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>15.789473684210526</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>13.5</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F5">
+        <f>19</f>
+        <v>19</v>
+      </c>
+      <c r="G5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H5">
+        <f>G5/F5*100</f>
+        <v>21.052631578947366</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:E6" si="2">D5+1</f>
+        <v>14.5</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
+      <c r="F6">
+        <f>19</f>
+        <v>19</v>
+      </c>
+      <c r="G6">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <f>G6/F6*100</f>
+        <v>5.2631578947368416</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
+      <c r="D7">
+        <f t="shared" ref="D7:E7" si="3">D6+1</f>
+        <v>15.5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <f>19</f>
+        <v>19</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7:H7" si="4">G6+1</f>
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ref="H7:H8" si="5">G7/F7*100</f>
+        <v>10.526315789473683</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>5</v>
+      <c r="D8">
+        <f t="shared" ref="D8:E8" si="6">D7+1</f>
+        <v>16.5</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <f>19</f>
+        <v>19</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ref="G8:H8" si="7">G7+1</f>
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="5"/>
+        <v>15.789473684210526</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ref="D9:E9" si="8">D8+1</f>
+        <v>17.5</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <f>19</f>
+        <v>19</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ref="G9:H9" si="9">G8+1</f>
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <f>G9/F9*100</f>
+        <v>21.052631578947366</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Filled In Current Data
Filled in the graphs with the current experiment data. Still need more.
</commit_message>
<xml_diff>
--- a/imports/vpl-fnl_pjt_data.xlsx
+++ b/imports/vpl-fnl_pjt_data.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roder\source\year 4 repos\HCI-FNL_PJT\imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45C2502-05EA-4CBC-81EA-D49BE157EF54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C97652-7D20-43A6-A1A1-54FFB4C51591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{648EF0DD-0358-465E-A7D1-701403DC3CB5}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="7500" windowHeight="11112" xr2:uid="{648EF0DD-0358-465E-A7D1-701403DC3CB5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Results" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="12">
   <si>
     <t>Participant</t>
   </si>
@@ -76,7 +76,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,12 +92,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -102,14 +115,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -421,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73DA4086-D66D-4A32-8F38-A033B2F7B296}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -473,22 +490,20 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>10.5</v>
+        <v>31.895</v>
       </c>
       <c r="E2">
-        <f>1</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2">
-        <f>1</f>
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <f>G2/F2*100</f>
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="H2" s="2">
+        <f>G2/F2</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -502,23 +517,20 @@
         <v>5</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:G5" si="0">D2+1</f>
-        <v>11.5</v>
+        <v>102.792</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F3">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="G3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H4" si="1">G3/F3*100</f>
-        <v>13.333333333333334</v>
+        <v>5</v>
+      </c>
+      <c r="H3" s="2">
+        <f>G3/F3</f>
+        <v>0.14285714285714285</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -526,30 +538,26 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>12.5</v>
+        <v>144.64099999999999</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F4">
-        <f>19</f>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="1"/>
-        <v>15.789473684210526</v>
+        <v>16</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" ref="H4:H9" si="0">G4/F4</f>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -557,30 +565,26 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5">
+        <v>35.966999999999999</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5" s="2">
         <f t="shared" si="0"/>
-        <v>13.5</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <f>19</f>
-        <v>19</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H5">
-        <f>G5/F5*100</f>
-        <v>21.052631578947366</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -594,24 +598,20 @@
         <v>4</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:E6" si="2">D5+1</f>
-        <v>14.5</v>
+        <v>83.334000000000003</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F6">
-        <f>19</f>
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G6">
-        <f>1</f>
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <f>G6/F6*100</f>
-        <v>5.2631578947368416</v>
+        <v>12</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -625,24 +625,20 @@
         <v>5</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:E7" si="3">D6+1</f>
-        <v>15.5</v>
+        <v>240.61199999999999</v>
       </c>
       <c r="E7">
-        <f t="shared" si="3"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F7">
-        <f>19</f>
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G7">
-        <f t="shared" ref="G7:H7" si="4">G6+1</f>
-        <v>2</v>
-      </c>
-      <c r="H7">
-        <f t="shared" ref="H7:H8" si="5">G7/F7*100</f>
-        <v>10.526315789473683</v>
+        <v>10</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -650,30 +646,26 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:E8" si="6">D7+1</f>
-        <v>16.5</v>
+        <v>47.143000000000001</v>
       </c>
       <c r="E8">
-        <f t="shared" si="6"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F8">
-        <f>19</f>
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:H8" si="7">G7+1</f>
-        <v>3</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="5"/>
-        <v>15.789473684210526</v>
+        <v>9</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -681,30 +673,264 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9:E9" si="8">D8+1</f>
+        <v>64.253</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="E10" s="1">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>10</v>
+      </c>
+      <c r="G10" s="1">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <f>G10/F10*100</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1">
+        <f>D10+2</f>
+        <v>12.5</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" ref="D11:G13" si="1">E10+1</f>
+        <v>2</v>
+      </c>
+      <c r="F11" s="1">
+        <v>15</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" ref="H11:H12" si="2">G11/F11*100</f>
+        <v>13.333333333333334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="1"/>
+        <v>13.5</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F12" s="1">
+        <v>25</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="1"/>
+        <v>14.5</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F13" s="1">
+        <v>30</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H13" s="1">
+        <f>G13/F13*100</f>
+        <v>13.333333333333334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" ref="D14:E14" si="3">D13+1</f>
+        <v>15.5</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="F14" s="1">
+        <v>53</v>
+      </c>
+      <c r="G14" s="1">
+        <v>2</v>
+      </c>
+      <c r="H14" s="1">
+        <f>G14/F14*100</f>
+        <v>3.7735849056603774</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" ref="D15:E15" si="4">D14+1</f>
+        <v>16.5</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="F15" s="1">
+        <v>7</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" ref="G15" si="5">G14+1</f>
+        <v>3</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" ref="H15:H16" si="6">G15/F15*100</f>
+        <v>42.857142857142854</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" ref="D16:E16" si="7">D15+1</f>
         <v>17.5</v>
       </c>
-      <c r="E9">
-        <f t="shared" si="8"/>
+      <c r="E16" s="1">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="F16" s="1">
+        <v>5</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" ref="G16" si="8">G15+1</f>
+        <v>4</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="6"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
         <v>8</v>
       </c>
-      <c r="F9">
-        <f>19</f>
-        <v>19</v>
-      </c>
-      <c r="G9">
-        <f t="shared" ref="G9:H9" si="9">G8+1</f>
-        <v>4</v>
-      </c>
-      <c r="H9">
-        <f>G9/F9*100</f>
-        <v>21.052631578947366</v>
+      <c r="B17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" ref="D17:E17" si="9">D16+1</f>
+        <v>18.5</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="F17" s="1">
+        <v>10</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" ref="G17" si="10">G16+1</f>
+        <v>5</v>
+      </c>
+      <c r="H17" s="1">
+        <f>G17/F17*100</f>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Just manaully exported some images.
I manually exported some image since I didn't have the automatic system setup. Will replace them later.
</commit_message>
<xml_diff>
--- a/imports/vpl-fnl_pjt_data.xlsx
+++ b/imports/vpl-fnl_pjt_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roder\source\year 4 repos\HCI-FNL_PJT\imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF2259B-55D8-401E-AB82-D5AE7657F6B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56A9A5C-8828-48CC-AE01-4C47EFC0A6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{648EF0DD-0358-465E-A7D1-701403DC3CB5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{648EF0DD-0358-465E-A7D1-701403DC3CB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -561,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73DA4086-D66D-4A32-8F38-A033B2F7B296}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -827,22 +827,20 @@
         <v>5</v>
       </c>
       <c r="D10" s="1">
-        <v>10.5</v>
+        <v>36.023000000000003</v>
       </c>
       <c r="E10" s="1">
-        <f>1</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F10" s="1">
         <v>10</v>
       </c>
       <c r="G10" s="1">
-        <f>1</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H10" s="1">
         <f>G10/F10*100</f>
-        <v>10</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -856,23 +854,20 @@
         <v>4</v>
       </c>
       <c r="D11" s="1">
-        <f>D10+2</f>
-        <v>12.5</v>
+        <v>31.962</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" ref="D11:G13" si="1">E10+1</f>
         <v>2</v>
       </c>
       <c r="F11" s="1">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" ref="H11:H12" si="2">G11/F11*100</f>
-        <v>13.333333333333334</v>
+        <f t="shared" ref="H11:H12" si="1">G11/F11*100</f>
+        <v>16.666666666666664</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -886,22 +881,20 @@
         <v>5</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="1"/>
-        <v>13.5</v>
+        <v>58.320999999999998</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="F12" s="1">
         <v>25</v>
       </c>
       <c r="G12" s="1">
+        <f t="shared" ref="D11:G13" si="2">G11+1</f>
+        <v>3</v>
+      </c>
+      <c r="H12" s="1">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="H12" s="1">
-        <f t="shared" si="2"/>
         <v>12</v>
       </c>
     </row>
@@ -916,23 +909,20 @@
         <v>4</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="1"/>
-        <v>14.5</v>
+        <v>24.635000000000002</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F13" s="1">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H13" s="1">
         <f>G13/F13*100</f>
-        <v>13.333333333333334</v>
+        <v>36.84210526315789</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -946,22 +936,20 @@
         <v>5</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" ref="D14:E14" si="3">D13+1</f>
-        <v>15.5</v>
+        <v>50.241999999999997</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F14" s="1">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="G14" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H14" s="1">
         <f>G14/F14*100</f>
-        <v>3.7735849056603774</v>
+        <v>22.222222222222221</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -975,23 +963,20 @@
         <v>4</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" ref="D15:E15" si="4">D14+1</f>
-        <v>16.5</v>
+        <v>80.125</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="4"/>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F15" s="1">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" ref="G15" si="5">G14+1</f>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" ref="H15:H16" si="6">G15/F15*100</f>
-        <v>42.857142857142854</v>
+        <f t="shared" ref="H15:H16" si="3">G15/F15*100</f>
+        <v>61.904761904761905</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1005,23 +990,20 @@
         <v>5</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" ref="D16:E16" si="7">D15+1</f>
-        <v>17.5</v>
+        <v>65.521000000000001</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="7"/>
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F16" s="1">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" ref="G16" si="8">G15+1</f>
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="6"/>
-        <v>80</v>
+        <f t="shared" si="3"/>
+        <v>71.428571428571431</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1035,23 +1017,22 @@
         <v>4</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" ref="D17:E17" si="9">D16+1</f>
-        <v>18.5</v>
+        <v>72.513999999999996</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" si="9"/>
-        <v>8</v>
+        <f t="shared" ref="D17:E17" si="4">E16+1</f>
+        <v>21</v>
       </c>
       <c r="F17" s="1">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" ref="G17" si="10">G16+1</f>
-        <v>5</v>
+        <f t="shared" ref="G17" si="5">G16+1</f>
+        <v>21</v>
       </c>
       <c r="H17" s="1">
         <f>G17/F17*100</f>
-        <v>50</v>
+        <v>52.5</v>
       </c>
     </row>
   </sheetData>
@@ -1063,7 +1044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAD3DC0-0BAB-4632-81BA-A01285DC1771}">
   <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+    <sheetView topLeftCell="A185" workbookViewId="0">
       <selection activeCell="K201" sqref="K201"/>
     </sheetView>
   </sheetViews>
@@ -1118,7 +1099,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
-        <f t="shared" ref="A4:A12" si="0">A3+1</f>
+        <f t="shared" ref="A4:A11" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -4589,7 +4570,7 @@
         <v>10</v>
       </c>
       <c r="B21" t="str">
-        <f t="shared" ref="B12:B21" si="2">B15</f>
+        <f t="shared" ref="B21" si="2">B15</f>
         <v>01. I feel accomplished?</v>
       </c>
       <c r="C21" t="s">

</xml_diff>

<commit_message>
Entered in Game Data. Still Need to Enter Questionnaire Data.
I've entered in the game data, but I still need to enter in the data from the questionnaires.
</commit_message>
<xml_diff>
--- a/imports/vpl-fnl_pjt_data.xlsx
+++ b/imports/vpl-fnl_pjt_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roder\source\year 4 repos\HCI-FNL_PJT\imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56A9A5C-8828-48CC-AE01-4C47EFC0A6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7858AC0D-2256-411B-BEBC-8A21F9C3EC6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{648EF0DD-0358-465E-A7D1-701403DC3CB5}"/>
+    <workbookView xWindow="12048" yWindow="1032" windowWidth="7500" windowHeight="11112" activeTab="3" xr2:uid="{648EF0DD-0358-465E-A7D1-701403DC3CB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="50">
   <si>
     <t>Participant</t>
   </si>
@@ -129,24 +129,6 @@
     <t>10. I needed to learn a lot of things before I could get going with this system.</t>
   </si>
   <si>
-    <t>01. I feel accomplished?</t>
-  </si>
-  <si>
-    <t>02. I feel happy?</t>
-  </si>
-  <si>
-    <t>03. I feel like I could have done more?</t>
-  </si>
-  <si>
-    <t>04. I felt frustrated?</t>
-  </si>
-  <si>
-    <t>05. I felt that I wasted my time?</t>
-  </si>
-  <si>
-    <t>06. I felt exhausted?</t>
-  </si>
-  <si>
     <t>01. I think that I would like to use this system frequently.</t>
   </si>
   <si>
@@ -172,6 +154,39 @@
   </si>
   <si>
     <t>09. I felt very confident using the system.</t>
+  </si>
+  <si>
+    <t>01. I enjoyed playing the game.</t>
+  </si>
+  <si>
+    <t>02. Overall, I feel that I am good at the game.</t>
+  </si>
+  <si>
+    <t>03. I feel that I improved the longer I played the game.</t>
+  </si>
+  <si>
+    <t>04. Overall, I felt I understood what I was doing in the game.</t>
+  </si>
+  <si>
+    <t>05. I felt time pressured (the timer factored into how I played the game).</t>
+  </si>
+  <si>
+    <t>06. I felt tense playing the game most of the time.</t>
+  </si>
+  <si>
+    <t>07. I felt the game was challenging.</t>
+  </si>
+  <si>
+    <t>08. I felt the failures were my fault, not the game’s fault.</t>
+  </si>
+  <si>
+    <t>Scores marked with a -1 have not been set, and in R will be turned into a 0.</t>
+  </si>
+  <si>
+    <t>Scores marked with a -1 are not available, and in R will be turned into a 0.</t>
+  </si>
+  <si>
+    <t>When the questions are asked, they are given in a 1 to 5 scale, so make sure to convert it to a 0 to 4 scale (i.e. x' = x - 1) for data entries.</t>
   </si>
 </sst>
 </file>
@@ -559,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73DA4086-D66D-4A32-8F38-A033B2F7B296}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -677,7 +692,7 @@
         <v>16</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" ref="H4:H9" si="0">G4/F4</f>
+        <f t="shared" ref="H4:H21" si="0">G4/F4</f>
         <v>1</v>
       </c>
     </row>
@@ -821,10 +836,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1">
         <v>36.023000000000003</v>
@@ -848,10 +863,10 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D11" s="1">
         <v>31.962</v>
@@ -866,174 +881,389 @@
         <v>2</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" ref="H11:H12" si="1">G11/F11*100</f>
+        <f t="shared" ref="H11" si="1">G11/F11*100</f>
         <v>16.666666666666664</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+      <c r="A12">
         <v>6</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="1">
-        <v>58.320999999999998</v>
-      </c>
-      <c r="E12" s="1">
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>50.634</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <v>71</v>
+      </c>
+      <c r="G12">
+        <v>15</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.21126760563380281</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="1">
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>27.974</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>36</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="0"/>
+        <v>2.7777777777777776E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>15.811</v>
+      </c>
+      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <v>7</v>
+      </c>
+      <c r="G14">
+        <v>7</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>12.699</v>
+      </c>
+      <c r="E15">
+        <v>8</v>
+      </c>
+      <c r="F15">
+        <v>8</v>
+      </c>
+      <c r="G15">
+        <v>8</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>28.516999999999999</v>
+      </c>
+      <c r="E16">
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <v>7</v>
+      </c>
+      <c r="G16">
+        <v>7</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>22.797000000000001</v>
+      </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <v>7</v>
+      </c>
+      <c r="G17">
+        <v>7</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>24.518000000000001</v>
+      </c>
+      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="F18">
         <v>25</v>
       </c>
-      <c r="G12" s="1">
-        <f t="shared" ref="D11:G13" si="2">G11+1</f>
+      <c r="G18">
+        <v>7</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="0"/>
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
         <v>3</v>
       </c>
-      <c r="H12" s="1">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>6</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>28.576000000000001</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>23.035</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="1">
-        <v>24.635000000000002</v>
-      </c>
-      <c r="E13" s="1">
-        <v>7</v>
-      </c>
-      <c r="F13" s="1">
-        <v>19</v>
-      </c>
-      <c r="G13" s="1">
-        <v>7</v>
-      </c>
-      <c r="H13" s="1">
-        <f>G13/F13*100</f>
-        <v>36.84210526315789</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>7</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="1">
-        <v>50.241999999999997</v>
-      </c>
-      <c r="E14" s="1">
-        <v>6</v>
-      </c>
-      <c r="F14" s="1">
-        <v>27</v>
-      </c>
-      <c r="G14" s="1">
-        <v>6</v>
-      </c>
-      <c r="H14" s="1">
-        <f>G14/F14*100</f>
-        <v>22.222222222222221</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>7</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="1">
-        <v>80.125</v>
-      </c>
-      <c r="E15" s="1">
-        <v>13</v>
-      </c>
-      <c r="F15" s="1">
-        <v>21</v>
-      </c>
-      <c r="G15" s="1">
-        <v>13</v>
-      </c>
-      <c r="H15" s="1">
-        <f t="shared" ref="H15:H16" si="3">G15/F15*100</f>
-        <v>61.904761904761905</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>8</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="1">
-        <v>65.521000000000001</v>
-      </c>
-      <c r="E16" s="1">
-        <v>20</v>
-      </c>
-      <c r="F16" s="1">
-        <v>28</v>
-      </c>
-      <c r="G16" s="1">
-        <v>20</v>
-      </c>
-      <c r="H16" s="1">
-        <f t="shared" si="3"/>
-        <v>71.428571428571431</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>8</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="1">
-        <v>72.513999999999996</v>
-      </c>
-      <c r="E17" s="1">
-        <f t="shared" ref="D17:E17" si="4">E16+1</f>
-        <v>21</v>
-      </c>
-      <c r="F17" s="1">
-        <v>40</v>
-      </c>
-      <c r="G17" s="1">
-        <f t="shared" ref="G17" si="5">G16+1</f>
-        <v>21</v>
-      </c>
-      <c r="H17" s="1">
-        <f>G17/F17*100</f>
-        <v>52.5</v>
-      </c>
+      <c r="D21">
+        <v>46.078000000000003</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>32</v>
+      </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15625</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1044,8 +1274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAD3DC0-0BAB-4632-81BA-A01285DC1771}">
   <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="K201" sqref="K201"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1073,7 +1303,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1088,7 +1318,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -1103,7 +1333,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1118,7 +1348,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1133,7 +1363,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1148,7 +1378,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -1163,7 +1393,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -1178,7 +1408,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1193,7 +1423,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -1208,7 +1438,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -1223,7 +1453,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -1238,7 +1468,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -1253,7 +1483,7 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -1268,7 +1498,7 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -1283,7 +1513,7 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -1298,7 +1528,7 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -1313,7 +1543,7 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
@@ -1328,7 +1558,7 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -1343,7 +1573,7 @@
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -1358,7 +1588,7 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -1373,7 +1603,7 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C22" t="str">
         <f>C2</f>
@@ -1389,7 +1619,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" ref="C23:C86" si="3">C3</f>
@@ -1405,7 +1635,7 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="3"/>
@@ -1421,7 +1651,7 @@
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="3"/>
@@ -1437,7 +1667,7 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="3"/>
@@ -1453,7 +1683,7 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="3"/>
@@ -1469,7 +1699,7 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="3"/>
@@ -1485,7 +1715,7 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="3"/>
@@ -1501,7 +1731,7 @@
         <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="3"/>
@@ -1517,7 +1747,7 @@
         <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="3"/>
@@ -1533,7 +1763,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="3"/>
@@ -1549,7 +1779,7 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="3"/>
@@ -1565,7 +1795,7 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="3"/>
@@ -1581,7 +1811,7 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="3"/>
@@ -1597,7 +1827,7 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="3"/>
@@ -1613,7 +1843,7 @@
         <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="3"/>
@@ -1629,7 +1859,7 @@
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="3"/>
@@ -1645,7 +1875,7 @@
         <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="3"/>
@@ -1661,7 +1891,7 @@
         <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="3"/>
@@ -1677,7 +1907,7 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="3"/>
@@ -1693,7 +1923,7 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="3"/>
@@ -1709,7 +1939,7 @@
         <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="3"/>
@@ -1725,7 +1955,7 @@
         <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="3"/>
@@ -1741,7 +1971,7 @@
         <v>4</v>
       </c>
       <c r="B45" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="3"/>
@@ -1757,7 +1987,7 @@
         <v>5</v>
       </c>
       <c r="B46" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="3"/>
@@ -1773,7 +2003,7 @@
         <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="3"/>
@@ -1789,7 +2019,7 @@
         <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="3"/>
@@ -1805,7 +2035,7 @@
         <v>8</v>
       </c>
       <c r="B49" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="3"/>
@@ -1821,7 +2051,7 @@
         <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="3"/>
@@ -1837,7 +2067,7 @@
         <v>10</v>
       </c>
       <c r="B51" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="3"/>
@@ -1853,7 +2083,7 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="3"/>
@@ -1869,7 +2099,7 @@
         <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="3"/>
@@ -1885,7 +2115,7 @@
         <v>3</v>
       </c>
       <c r="B54" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="3"/>
@@ -1901,7 +2131,7 @@
         <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="3"/>
@@ -1917,7 +2147,7 @@
         <v>5</v>
       </c>
       <c r="B56" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="3"/>
@@ -1933,7 +2163,7 @@
         <v>6</v>
       </c>
       <c r="B57" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="3"/>
@@ -1949,7 +2179,7 @@
         <v>7</v>
       </c>
       <c r="B58" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="3"/>
@@ -1965,7 +2195,7 @@
         <v>8</v>
       </c>
       <c r="B59" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="3"/>
@@ -1981,7 +2211,7 @@
         <v>9</v>
       </c>
       <c r="B60" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="3"/>
@@ -1997,7 +2227,7 @@
         <v>10</v>
       </c>
       <c r="B61" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="3"/>
@@ -2013,7 +2243,7 @@
         <v>1</v>
       </c>
       <c r="B62" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="3"/>
@@ -2029,7 +2259,7 @@
         <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="3"/>
@@ -2045,7 +2275,7 @@
         <v>3</v>
       </c>
       <c r="B64" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="3"/>
@@ -2061,7 +2291,7 @@
         <v>4</v>
       </c>
       <c r="B65" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="3"/>
@@ -2077,7 +2307,7 @@
         <v>5</v>
       </c>
       <c r="B66" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="3"/>
@@ -2093,7 +2323,7 @@
         <v>6</v>
       </c>
       <c r="B67" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" si="3"/>
@@ -2109,7 +2339,7 @@
         <v>7</v>
       </c>
       <c r="B68" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="3"/>
@@ -2125,7 +2355,7 @@
         <v>8</v>
       </c>
       <c r="B69" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="3"/>
@@ -2141,7 +2371,7 @@
         <v>9</v>
       </c>
       <c r="B70" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="3"/>
@@ -2157,7 +2387,7 @@
         <v>10</v>
       </c>
       <c r="B71" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="3"/>
@@ -2173,7 +2403,7 @@
         <v>1</v>
       </c>
       <c r="B72" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="3"/>
@@ -2189,7 +2419,7 @@
         <v>2</v>
       </c>
       <c r="B73" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="3"/>
@@ -2205,7 +2435,7 @@
         <v>3</v>
       </c>
       <c r="B74" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="3"/>
@@ -2221,7 +2451,7 @@
         <v>4</v>
       </c>
       <c r="B75" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="3"/>
@@ -2237,7 +2467,7 @@
         <v>5</v>
       </c>
       <c r="B76" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="3"/>
@@ -2253,7 +2483,7 @@
         <v>6</v>
       </c>
       <c r="B77" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="3"/>
@@ -2269,7 +2499,7 @@
         <v>7</v>
       </c>
       <c r="B78" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="3"/>
@@ -2285,7 +2515,7 @@
         <v>8</v>
       </c>
       <c r="B79" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="3"/>
@@ -2301,7 +2531,7 @@
         <v>9</v>
       </c>
       <c r="B80" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C80" t="str">
         <f t="shared" si="3"/>
@@ -2317,7 +2547,7 @@
         <v>10</v>
       </c>
       <c r="B81" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C81" t="str">
         <f t="shared" si="3"/>
@@ -2333,7 +2563,7 @@
         <v>1</v>
       </c>
       <c r="B82" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C82" t="str">
         <f t="shared" si="3"/>
@@ -2349,7 +2579,7 @@
         <v>2</v>
       </c>
       <c r="B83" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C83" t="str">
         <f t="shared" si="3"/>
@@ -2365,7 +2595,7 @@
         <v>3</v>
       </c>
       <c r="B84" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="3"/>
@@ -2381,7 +2611,7 @@
         <v>4</v>
       </c>
       <c r="B85" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="3"/>
@@ -2397,7 +2627,7 @@
         <v>5</v>
       </c>
       <c r="B86" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="3"/>
@@ -2413,7 +2643,7 @@
         <v>6</v>
       </c>
       <c r="B87" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" ref="C87:C150" si="5">C67</f>
@@ -2429,7 +2659,7 @@
         <v>7</v>
       </c>
       <c r="B88" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C88" t="str">
         <f t="shared" si="5"/>
@@ -2445,7 +2675,7 @@
         <v>8</v>
       </c>
       <c r="B89" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="5"/>
@@ -2461,7 +2691,7 @@
         <v>9</v>
       </c>
       <c r="B90" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="5"/>
@@ -2477,7 +2707,7 @@
         <v>10</v>
       </c>
       <c r="B91" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="5"/>
@@ -2493,7 +2723,7 @@
         <v>1</v>
       </c>
       <c r="B92" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="5"/>
@@ -2509,7 +2739,7 @@
         <v>2</v>
       </c>
       <c r="B93" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="5"/>
@@ -2525,7 +2755,7 @@
         <v>3</v>
       </c>
       <c r="B94" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="5"/>
@@ -2541,7 +2771,7 @@
         <v>4</v>
       </c>
       <c r="B95" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="5"/>
@@ -2557,7 +2787,7 @@
         <v>5</v>
       </c>
       <c r="B96" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="5"/>
@@ -2573,7 +2803,7 @@
         <v>6</v>
       </c>
       <c r="B97" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="5"/>
@@ -2589,7 +2819,7 @@
         <v>7</v>
       </c>
       <c r="B98" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C98" t="str">
         <f t="shared" si="5"/>
@@ -2605,7 +2835,7 @@
         <v>8</v>
       </c>
       <c r="B99" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C99" t="str">
         <f t="shared" si="5"/>
@@ -2621,7 +2851,7 @@
         <v>9</v>
       </c>
       <c r="B100" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C100" t="str">
         <f t="shared" si="5"/>
@@ -2637,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="B101" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C101" t="str">
         <f t="shared" si="5"/>
@@ -2653,7 +2883,7 @@
         <v>1</v>
       </c>
       <c r="B102" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C102" t="str">
         <f t="shared" si="5"/>
@@ -2669,7 +2899,7 @@
         <v>2</v>
       </c>
       <c r="B103" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C103" t="str">
         <f t="shared" si="5"/>
@@ -2685,7 +2915,7 @@
         <v>3</v>
       </c>
       <c r="B104" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C104" t="str">
         <f t="shared" si="5"/>
@@ -2701,7 +2931,7 @@
         <v>4</v>
       </c>
       <c r="B105" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C105" t="str">
         <f t="shared" si="5"/>
@@ -2717,7 +2947,7 @@
         <v>5</v>
       </c>
       <c r="B106" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C106" t="str">
         <f t="shared" si="5"/>
@@ -2733,7 +2963,7 @@
         <v>6</v>
       </c>
       <c r="B107" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C107" t="str">
         <f t="shared" si="5"/>
@@ -2749,7 +2979,7 @@
         <v>7</v>
       </c>
       <c r="B108" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C108" t="str">
         <f t="shared" si="5"/>
@@ -2765,7 +2995,7 @@
         <v>8</v>
       </c>
       <c r="B109" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C109" t="str">
         <f t="shared" si="5"/>
@@ -2781,7 +3011,7 @@
         <v>9</v>
       </c>
       <c r="B110" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C110" t="str">
         <f t="shared" si="5"/>
@@ -2797,7 +3027,7 @@
         <v>10</v>
       </c>
       <c r="B111" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C111" t="str">
         <f t="shared" si="5"/>
@@ -2813,7 +3043,7 @@
         <v>1</v>
       </c>
       <c r="B112" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C112" t="str">
         <f t="shared" si="5"/>
@@ -2829,7 +3059,7 @@
         <v>2</v>
       </c>
       <c r="B113" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C113" t="str">
         <f t="shared" si="5"/>
@@ -2845,7 +3075,7 @@
         <v>3</v>
       </c>
       <c r="B114" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C114" t="str">
         <f t="shared" si="5"/>
@@ -2861,7 +3091,7 @@
         <v>4</v>
       </c>
       <c r="B115" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C115" t="str">
         <f t="shared" si="5"/>
@@ -2877,7 +3107,7 @@
         <v>5</v>
       </c>
       <c r="B116" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C116" t="str">
         <f t="shared" si="5"/>
@@ -2893,7 +3123,7 @@
         <v>6</v>
       </c>
       <c r="B117" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C117" t="str">
         <f t="shared" si="5"/>
@@ -2909,7 +3139,7 @@
         <v>7</v>
       </c>
       <c r="B118" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C118" t="str">
         <f t="shared" si="5"/>
@@ -2925,7 +3155,7 @@
         <v>8</v>
       </c>
       <c r="B119" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C119" t="str">
         <f t="shared" si="5"/>
@@ -2941,7 +3171,7 @@
         <v>9</v>
       </c>
       <c r="B120" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C120" t="str">
         <f t="shared" si="5"/>
@@ -2957,7 +3187,7 @@
         <v>10</v>
       </c>
       <c r="B121" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C121" t="str">
         <f t="shared" si="5"/>
@@ -2973,7 +3203,7 @@
         <v>1</v>
       </c>
       <c r="B122" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C122" t="str">
         <f t="shared" si="5"/>
@@ -2989,7 +3219,7 @@
         <v>2</v>
       </c>
       <c r="B123" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C123" t="str">
         <f t="shared" si="5"/>
@@ -3005,7 +3235,7 @@
         <v>3</v>
       </c>
       <c r="B124" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C124" t="str">
         <f t="shared" si="5"/>
@@ -3021,7 +3251,7 @@
         <v>4</v>
       </c>
       <c r="B125" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C125" t="str">
         <f t="shared" si="5"/>
@@ -3037,7 +3267,7 @@
         <v>5</v>
       </c>
       <c r="B126" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C126" t="str">
         <f t="shared" si="5"/>
@@ -3053,7 +3283,7 @@
         <v>6</v>
       </c>
       <c r="B127" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C127" t="str">
         <f t="shared" si="5"/>
@@ -3069,7 +3299,7 @@
         <v>7</v>
       </c>
       <c r="B128" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C128" t="str">
         <f t="shared" si="5"/>
@@ -3085,7 +3315,7 @@
         <v>8</v>
       </c>
       <c r="B129" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C129" t="str">
         <f t="shared" si="5"/>
@@ -3101,7 +3331,7 @@
         <v>9</v>
       </c>
       <c r="B130" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C130" t="str">
         <f t="shared" si="5"/>
@@ -3117,7 +3347,7 @@
         <v>10</v>
       </c>
       <c r="B131" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C131" t="str">
         <f t="shared" si="5"/>
@@ -3133,7 +3363,7 @@
         <v>1</v>
       </c>
       <c r="B132" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C132" t="str">
         <f t="shared" si="5"/>
@@ -3149,7 +3379,7 @@
         <v>2</v>
       </c>
       <c r="B133" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C133" t="str">
         <f t="shared" si="5"/>
@@ -3165,7 +3395,7 @@
         <v>3</v>
       </c>
       <c r="B134" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C134" t="str">
         <f t="shared" si="5"/>
@@ -3181,7 +3411,7 @@
         <v>4</v>
       </c>
       <c r="B135" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C135" t="str">
         <f t="shared" si="5"/>
@@ -3197,7 +3427,7 @@
         <v>5</v>
       </c>
       <c r="B136" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C136" t="str">
         <f t="shared" si="5"/>
@@ -3213,7 +3443,7 @@
         <v>6</v>
       </c>
       <c r="B137" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C137" t="str">
         <f t="shared" si="5"/>
@@ -3229,7 +3459,7 @@
         <v>7</v>
       </c>
       <c r="B138" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C138" t="str">
         <f t="shared" si="5"/>
@@ -3245,7 +3475,7 @@
         <v>8</v>
       </c>
       <c r="B139" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C139" t="str">
         <f t="shared" si="5"/>
@@ -3261,7 +3491,7 @@
         <v>9</v>
       </c>
       <c r="B140" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C140" t="str">
         <f t="shared" si="5"/>
@@ -3277,7 +3507,7 @@
         <v>10</v>
       </c>
       <c r="B141" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C141" t="str">
         <f t="shared" si="5"/>
@@ -3293,7 +3523,7 @@
         <v>1</v>
       </c>
       <c r="B142" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C142" t="str">
         <f t="shared" si="5"/>
@@ -3309,7 +3539,7 @@
         <v>2</v>
       </c>
       <c r="B143" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C143" t="str">
         <f t="shared" si="5"/>
@@ -3325,7 +3555,7 @@
         <v>3</v>
       </c>
       <c r="B144" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C144" t="str">
         <f t="shared" si="5"/>
@@ -3341,7 +3571,7 @@
         <v>4</v>
       </c>
       <c r="B145" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C145" t="str">
         <f t="shared" si="5"/>
@@ -3357,7 +3587,7 @@
         <v>5</v>
       </c>
       <c r="B146" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C146" t="str">
         <f t="shared" si="5"/>
@@ -3373,7 +3603,7 @@
         <v>6</v>
       </c>
       <c r="B147" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C147" t="str">
         <f t="shared" si="5"/>
@@ -3389,7 +3619,7 @@
         <v>7</v>
       </c>
       <c r="B148" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C148" t="str">
         <f t="shared" si="5"/>
@@ -3405,7 +3635,7 @@
         <v>8</v>
       </c>
       <c r="B149" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C149" t="str">
         <f t="shared" si="5"/>
@@ -3421,7 +3651,7 @@
         <v>9</v>
       </c>
       <c r="B150" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C150" t="str">
         <f t="shared" si="5"/>
@@ -3437,7 +3667,7 @@
         <v>10</v>
       </c>
       <c r="B151" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C151" t="str">
         <f t="shared" ref="C151:C201" si="7">C131</f>
@@ -3453,7 +3683,7 @@
         <v>1</v>
       </c>
       <c r="B152" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C152" t="str">
         <f t="shared" si="7"/>
@@ -3469,7 +3699,7 @@
         <v>2</v>
       </c>
       <c r="B153" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C153" t="str">
         <f t="shared" si="7"/>
@@ -3485,7 +3715,7 @@
         <v>3</v>
       </c>
       <c r="B154" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C154" t="str">
         <f t="shared" si="7"/>
@@ -3501,7 +3731,7 @@
         <v>4</v>
       </c>
       <c r="B155" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C155" t="str">
         <f t="shared" si="7"/>
@@ -3517,7 +3747,7 @@
         <v>5</v>
       </c>
       <c r="B156" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C156" t="str">
         <f t="shared" si="7"/>
@@ -3533,7 +3763,7 @@
         <v>6</v>
       </c>
       <c r="B157" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C157" t="str">
         <f t="shared" si="7"/>
@@ -3549,7 +3779,7 @@
         <v>7</v>
       </c>
       <c r="B158" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C158" t="str">
         <f t="shared" si="7"/>
@@ -3565,7 +3795,7 @@
         <v>8</v>
       </c>
       <c r="B159" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C159" t="str">
         <f t="shared" si="7"/>
@@ -3581,7 +3811,7 @@
         <v>9</v>
       </c>
       <c r="B160" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C160" t="str">
         <f t="shared" si="7"/>
@@ -3597,7 +3827,7 @@
         <v>10</v>
       </c>
       <c r="B161" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C161" t="str">
         <f t="shared" si="7"/>
@@ -3613,7 +3843,7 @@
         <v>1</v>
       </c>
       <c r="B162" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C162" t="str">
         <f t="shared" si="7"/>
@@ -3629,7 +3859,7 @@
         <v>2</v>
       </c>
       <c r="B163" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C163" t="str">
         <f t="shared" si="7"/>
@@ -3645,7 +3875,7 @@
         <v>3</v>
       </c>
       <c r="B164" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C164" t="str">
         <f t="shared" si="7"/>
@@ -3661,7 +3891,7 @@
         <v>4</v>
       </c>
       <c r="B165" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C165" t="str">
         <f t="shared" si="7"/>
@@ -3677,7 +3907,7 @@
         <v>5</v>
       </c>
       <c r="B166" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C166" t="str">
         <f t="shared" si="7"/>
@@ -3693,7 +3923,7 @@
         <v>6</v>
       </c>
       <c r="B167" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C167" t="str">
         <f t="shared" si="7"/>
@@ -3709,7 +3939,7 @@
         <v>7</v>
       </c>
       <c r="B168" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C168" t="str">
         <f t="shared" si="7"/>
@@ -3725,7 +3955,7 @@
         <v>8</v>
       </c>
       <c r="B169" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C169" t="str">
         <f t="shared" si="7"/>
@@ -3741,7 +3971,7 @@
         <v>9</v>
       </c>
       <c r="B170" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C170" t="str">
         <f t="shared" si="7"/>
@@ -3757,7 +3987,7 @@
         <v>10</v>
       </c>
       <c r="B171" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C171" t="str">
         <f t="shared" si="7"/>
@@ -3773,7 +4003,7 @@
         <v>1</v>
       </c>
       <c r="B172" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C172" t="str">
         <f t="shared" si="7"/>
@@ -3789,7 +4019,7 @@
         <v>2</v>
       </c>
       <c r="B173" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C173" t="str">
         <f t="shared" si="7"/>
@@ -3805,7 +4035,7 @@
         <v>3</v>
       </c>
       <c r="B174" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C174" t="str">
         <f t="shared" si="7"/>
@@ -3821,7 +4051,7 @@
         <v>4</v>
       </c>
       <c r="B175" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C175" t="str">
         <f t="shared" si="7"/>
@@ -3837,7 +4067,7 @@
         <v>5</v>
       </c>
       <c r="B176" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C176" t="str">
         <f t="shared" si="7"/>
@@ -3853,7 +4083,7 @@
         <v>6</v>
       </c>
       <c r="B177" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C177" t="str">
         <f t="shared" si="7"/>
@@ -3869,7 +4099,7 @@
         <v>7</v>
       </c>
       <c r="B178" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C178" t="str">
         <f t="shared" si="7"/>
@@ -3885,7 +4115,7 @@
         <v>8</v>
       </c>
       <c r="B179" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C179" t="str">
         <f t="shared" si="7"/>
@@ -3901,7 +4131,7 @@
         <v>9</v>
       </c>
       <c r="B180" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C180" t="str">
         <f t="shared" si="7"/>
@@ -3917,7 +4147,7 @@
         <v>10</v>
       </c>
       <c r="B181" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C181" t="str">
         <f t="shared" si="7"/>
@@ -4254,16 +4484,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6155F0-D76B-402B-AB6F-C6589B98D823}">
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:D161"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="M119" sqref="M119"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -4285,7 +4515,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -4300,7 +4530,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -4315,7 +4545,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -4330,7 +4560,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -4345,7 +4575,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -4360,7 +4590,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -4375,7 +4605,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -4390,7 +4620,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -4405,7 +4635,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -4420,7 +4650,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -4435,7 +4665,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -4450,7 +4680,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -4465,7 +4695,7 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -4480,7 +4710,7 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -4495,7 +4725,7 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -4510,7 +4740,7 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -4525,7 +4755,7 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
@@ -4540,7 +4770,7 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -4555,7 +4785,7 @@
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -4571,7 +4801,7 @@
       </c>
       <c r="B21" t="str">
         <f t="shared" ref="B21" si="2">B15</f>
-        <v>01. I feel accomplished?</v>
+        <v>01. I enjoyed playing the game.</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -4586,7 +4816,7 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C22" t="str">
         <f>C2</f>
@@ -4602,7 +4832,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" ref="C23:C40" si="3">C3</f>
@@ -4618,7 +4848,7 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="3"/>
@@ -4634,7 +4864,7 @@
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="3"/>
@@ -4650,7 +4880,7 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="3"/>
@@ -4666,7 +4896,7 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="3"/>
@@ -4682,7 +4912,7 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="3"/>
@@ -4698,7 +4928,7 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="3"/>
@@ -4714,7 +4944,7 @@
         <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="3"/>
@@ -4730,7 +4960,7 @@
         <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="3"/>
@@ -4746,7 +4976,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="3"/>
@@ -4762,7 +4992,7 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="3"/>
@@ -4778,7 +5008,7 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="3"/>
@@ -4794,7 +5024,7 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="3"/>
@@ -4810,7 +5040,7 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="3"/>
@@ -4826,7 +5056,7 @@
         <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="3"/>
@@ -4842,7 +5072,7 @@
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="3"/>
@@ -4858,7 +5088,7 @@
         <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="3"/>
@@ -4874,7 +5104,7 @@
         <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="3"/>
@@ -4890,7 +5120,7 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C41" t="str">
         <f>C21</f>
@@ -4906,7 +5136,7 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" ref="C42:C105" si="4">C22</f>
@@ -4922,7 +5152,7 @@
         <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="4"/>
@@ -4938,7 +5168,7 @@
         <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="4"/>
@@ -4954,7 +5184,7 @@
         <v>4</v>
       </c>
       <c r="B45" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="4"/>
@@ -4970,7 +5200,7 @@
         <v>5</v>
       </c>
       <c r="B46" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="4"/>
@@ -4986,7 +5216,7 @@
         <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="4"/>
@@ -5002,7 +5232,7 @@
         <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="4"/>
@@ -5018,7 +5248,7 @@
         <v>8</v>
       </c>
       <c r="B49" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="4"/>
@@ -5034,7 +5264,7 @@
         <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="4"/>
@@ -5050,7 +5280,7 @@
         <v>10</v>
       </c>
       <c r="B51" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="4"/>
@@ -5066,7 +5296,7 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="4"/>
@@ -5082,7 +5312,7 @@
         <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="4"/>
@@ -5098,7 +5328,7 @@
         <v>3</v>
       </c>
       <c r="B54" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C54" t="str">
         <f>C34</f>
@@ -5114,7 +5344,7 @@
         <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="4"/>
@@ -5130,7 +5360,7 @@
         <v>5</v>
       </c>
       <c r="B56" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="4"/>
@@ -5146,7 +5376,7 @@
         <v>6</v>
       </c>
       <c r="B57" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="4"/>
@@ -5162,7 +5392,7 @@
         <v>7</v>
       </c>
       <c r="B58" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="4"/>
@@ -5178,7 +5408,7 @@
         <v>8</v>
       </c>
       <c r="B59" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="4"/>
@@ -5194,7 +5424,7 @@
         <v>9</v>
       </c>
       <c r="B60" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="4"/>
@@ -5210,7 +5440,7 @@
         <v>10</v>
       </c>
       <c r="B61" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="4"/>
@@ -5222,11 +5452,11 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
-        <f t="shared" ref="A62:A121" si="5">A52</f>
+        <f t="shared" ref="A62:A125" si="5">A52</f>
         <v>1</v>
       </c>
       <c r="B62" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="4"/>
@@ -5242,7 +5472,7 @@
         <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="4"/>
@@ -5258,7 +5488,7 @@
         <v>3</v>
       </c>
       <c r="B64" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="4"/>
@@ -5274,7 +5504,7 @@
         <v>4</v>
       </c>
       <c r="B65" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="4"/>
@@ -5290,7 +5520,7 @@
         <v>5</v>
       </c>
       <c r="B66" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="4"/>
@@ -5306,7 +5536,7 @@
         <v>6</v>
       </c>
       <c r="B67" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" si="4"/>
@@ -5322,7 +5552,7 @@
         <v>7</v>
       </c>
       <c r="B68" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="4"/>
@@ -5338,7 +5568,7 @@
         <v>8</v>
       </c>
       <c r="B69" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="4"/>
@@ -5354,7 +5584,7 @@
         <v>9</v>
       </c>
       <c r="B70" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="4"/>
@@ -5370,7 +5600,7 @@
         <v>10</v>
       </c>
       <c r="B71" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="4"/>
@@ -5386,7 +5616,7 @@
         <v>1</v>
       </c>
       <c r="B72" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="4"/>
@@ -5402,7 +5632,7 @@
         <v>2</v>
       </c>
       <c r="B73" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="4"/>
@@ -5418,7 +5648,7 @@
         <v>3</v>
       </c>
       <c r="B74" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="4"/>
@@ -5434,7 +5664,7 @@
         <v>4</v>
       </c>
       <c r="B75" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="4"/>
@@ -5450,7 +5680,7 @@
         <v>5</v>
       </c>
       <c r="B76" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="4"/>
@@ -5466,7 +5696,7 @@
         <v>6</v>
       </c>
       <c r="B77" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="4"/>
@@ -5482,7 +5712,7 @@
         <v>7</v>
       </c>
       <c r="B78" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="4"/>
@@ -5498,7 +5728,7 @@
         <v>8</v>
       </c>
       <c r="B79" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="4"/>
@@ -5514,7 +5744,7 @@
         <v>9</v>
       </c>
       <c r="B80" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C80" t="str">
         <f t="shared" si="4"/>
@@ -5530,7 +5760,7 @@
         <v>10</v>
       </c>
       <c r="B81" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C81" t="str">
         <f t="shared" si="4"/>
@@ -5546,7 +5776,7 @@
         <v>1</v>
       </c>
       <c r="B82" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C82" t="str">
         <f t="shared" si="4"/>
@@ -5562,7 +5792,7 @@
         <v>2</v>
       </c>
       <c r="B83" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C83" t="str">
         <f t="shared" si="4"/>
@@ -5578,7 +5808,7 @@
         <v>3</v>
       </c>
       <c r="B84" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="4"/>
@@ -5594,7 +5824,7 @@
         <v>4</v>
       </c>
       <c r="B85" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="4"/>
@@ -5610,7 +5840,7 @@
         <v>5</v>
       </c>
       <c r="B86" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="4"/>
@@ -5626,7 +5856,7 @@
         <v>6</v>
       </c>
       <c r="B87" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="4"/>
@@ -5642,7 +5872,7 @@
         <v>7</v>
       </c>
       <c r="B88" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C88" t="str">
         <f t="shared" si="4"/>
@@ -5658,7 +5888,7 @@
         <v>8</v>
       </c>
       <c r="B89" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="4"/>
@@ -5674,7 +5904,7 @@
         <v>9</v>
       </c>
       <c r="B90" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="4"/>
@@ -5690,7 +5920,7 @@
         <v>10</v>
       </c>
       <c r="B91" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="4"/>
@@ -5706,7 +5936,7 @@
         <v>1</v>
       </c>
       <c r="B92" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="4"/>
@@ -5722,7 +5952,7 @@
         <v>2</v>
       </c>
       <c r="B93" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="4"/>
@@ -5738,7 +5968,7 @@
         <v>3</v>
       </c>
       <c r="B94" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="4"/>
@@ -5754,7 +5984,7 @@
         <v>4</v>
       </c>
       <c r="B95" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="4"/>
@@ -5770,7 +6000,7 @@
         <v>5</v>
       </c>
       <c r="B96" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="4"/>
@@ -5786,7 +6016,7 @@
         <v>6</v>
       </c>
       <c r="B97" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="4"/>
@@ -5802,7 +6032,7 @@
         <v>7</v>
       </c>
       <c r="B98" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C98" t="str">
         <f t="shared" si="4"/>
@@ -5818,7 +6048,7 @@
         <v>8</v>
       </c>
       <c r="B99" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C99" t="str">
         <f t="shared" si="4"/>
@@ -5834,7 +6064,7 @@
         <v>9</v>
       </c>
       <c r="B100" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C100" t="str">
         <f t="shared" si="4"/>
@@ -5850,7 +6080,7 @@
         <v>10</v>
       </c>
       <c r="B101" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C101" t="str">
         <f t="shared" si="4"/>
@@ -5866,7 +6096,7 @@
         <v>1</v>
       </c>
       <c r="B102" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C102" t="str">
         <f t="shared" si="4"/>
@@ -5882,7 +6112,7 @@
         <v>2</v>
       </c>
       <c r="B103" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C103" t="str">
         <f t="shared" si="4"/>
@@ -5898,7 +6128,7 @@
         <v>3</v>
       </c>
       <c r="B104" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C104" t="str">
         <f t="shared" si="4"/>
@@ -5914,7 +6144,7 @@
         <v>4</v>
       </c>
       <c r="B105" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C105" t="str">
         <f t="shared" si="4"/>
@@ -5930,10 +6160,10 @@
         <v>5</v>
       </c>
       <c r="B106" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C106" t="str">
-        <f t="shared" ref="C106:C121" si="6">C86</f>
+        <f t="shared" ref="C106:C161" si="6">C86</f>
         <v>A</v>
       </c>
       <c r="D106">
@@ -5946,7 +6176,7 @@
         <v>6</v>
       </c>
       <c r="B107" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C107" t="str">
         <f t="shared" si="6"/>
@@ -5962,7 +6192,7 @@
         <v>7</v>
       </c>
       <c r="B108" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C108" t="str">
         <f t="shared" si="6"/>
@@ -5978,7 +6208,7 @@
         <v>8</v>
       </c>
       <c r="B109" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C109" t="str">
         <f t="shared" si="6"/>
@@ -5994,7 +6224,7 @@
         <v>9</v>
       </c>
       <c r="B110" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C110" t="str">
         <f t="shared" si="6"/>
@@ -6010,7 +6240,7 @@
         <v>10</v>
       </c>
       <c r="B111" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C111" t="str">
         <f t="shared" si="6"/>
@@ -6026,7 +6256,7 @@
         <v>1</v>
       </c>
       <c r="B112" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C112" t="str">
         <f t="shared" si="6"/>
@@ -6042,7 +6272,7 @@
         <v>2</v>
       </c>
       <c r="B113" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C113" t="str">
         <f t="shared" si="6"/>
@@ -6058,7 +6288,7 @@
         <v>3</v>
       </c>
       <c r="B114" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C114" t="str">
         <f t="shared" si="6"/>
@@ -6074,7 +6304,7 @@
         <v>4</v>
       </c>
       <c r="B115" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C115" t="str">
         <f t="shared" si="6"/>
@@ -6090,7 +6320,7 @@
         <v>5</v>
       </c>
       <c r="B116" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C116" t="str">
         <f t="shared" si="6"/>
@@ -6106,7 +6336,7 @@
         <v>6</v>
       </c>
       <c r="B117" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C117" t="str">
         <f t="shared" si="6"/>
@@ -6122,7 +6352,7 @@
         <v>7</v>
       </c>
       <c r="B118" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C118" t="str">
         <f t="shared" si="6"/>
@@ -6138,7 +6368,7 @@
         <v>8</v>
       </c>
       <c r="B119" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C119" t="str">
         <f t="shared" si="6"/>
@@ -6154,7 +6384,7 @@
         <v>9</v>
       </c>
       <c r="B120" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C120" t="str">
         <f t="shared" si="6"/>
@@ -6170,13 +6400,653 @@
         <v>10</v>
       </c>
       <c r="B121" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C121" t="str">
         <f t="shared" si="6"/>
         <v>B</v>
       </c>
       <c r="D121">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="B122" t="s">
+        <v>45</v>
+      </c>
+      <c r="C122" t="str">
+        <f t="shared" si="6"/>
+        <v>A</v>
+      </c>
+      <c r="D122">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="B123" t="s">
+        <v>45</v>
+      </c>
+      <c r="C123" t="str">
+        <f t="shared" si="6"/>
+        <v>A</v>
+      </c>
+      <c r="D123">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="B124" t="s">
+        <v>45</v>
+      </c>
+      <c r="C124" t="str">
+        <f t="shared" si="6"/>
+        <v>A</v>
+      </c>
+      <c r="D124">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="B125" t="s">
+        <v>45</v>
+      </c>
+      <c r="C125" t="str">
+        <f t="shared" si="6"/>
+        <v>A</v>
+      </c>
+      <c r="D125">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <f t="shared" ref="A126:A161" si="7">A116</f>
+        <v>5</v>
+      </c>
+      <c r="B126" t="s">
+        <v>45</v>
+      </c>
+      <c r="C126" t="str">
+        <f t="shared" si="6"/>
+        <v>A</v>
+      </c>
+      <c r="D126">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="B127" t="s">
+        <v>45</v>
+      </c>
+      <c r="C127" t="str">
+        <f t="shared" si="6"/>
+        <v>A</v>
+      </c>
+      <c r="D127">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="B128" t="s">
+        <v>45</v>
+      </c>
+      <c r="C128" t="str">
+        <f t="shared" si="6"/>
+        <v>A</v>
+      </c>
+      <c r="D128">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="B129" t="s">
+        <v>45</v>
+      </c>
+      <c r="C129" t="str">
+        <f t="shared" si="6"/>
+        <v>A</v>
+      </c>
+      <c r="D129">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="B130" t="s">
+        <v>45</v>
+      </c>
+      <c r="C130" t="str">
+        <f t="shared" si="6"/>
+        <v>A</v>
+      </c>
+      <c r="D130">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="B131" t="s">
+        <v>45</v>
+      </c>
+      <c r="C131" t="str">
+        <f t="shared" si="6"/>
+        <v>A</v>
+      </c>
+      <c r="D131">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="B132" t="s">
+        <v>45</v>
+      </c>
+      <c r="C132" t="str">
+        <f t="shared" si="6"/>
+        <v>B</v>
+      </c>
+      <c r="D132">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="B133" t="s">
+        <v>45</v>
+      </c>
+      <c r="C133" t="str">
+        <f t="shared" si="6"/>
+        <v>B</v>
+      </c>
+      <c r="D133">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="B134" t="s">
+        <v>45</v>
+      </c>
+      <c r="C134" t="str">
+        <f t="shared" si="6"/>
+        <v>B</v>
+      </c>
+      <c r="D134">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="B135" t="s">
+        <v>45</v>
+      </c>
+      <c r="C135" t="str">
+        <f t="shared" si="6"/>
+        <v>B</v>
+      </c>
+      <c r="D135">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="B136" t="s">
+        <v>45</v>
+      </c>
+      <c r="C136" t="str">
+        <f t="shared" si="6"/>
+        <v>B</v>
+      </c>
+      <c r="D136">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="B137" t="s">
+        <v>45</v>
+      </c>
+      <c r="C137" t="str">
+        <f t="shared" si="6"/>
+        <v>B</v>
+      </c>
+      <c r="D137">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="B138" t="s">
+        <v>45</v>
+      </c>
+      <c r="C138" t="str">
+        <f t="shared" si="6"/>
+        <v>B</v>
+      </c>
+      <c r="D138">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="B139" t="s">
+        <v>45</v>
+      </c>
+      <c r="C139" t="str">
+        <f t="shared" si="6"/>
+        <v>B</v>
+      </c>
+      <c r="D139">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="B140" t="s">
+        <v>45</v>
+      </c>
+      <c r="C140" t="str">
+        <f t="shared" si="6"/>
+        <v>B</v>
+      </c>
+      <c r="D140">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="B141" t="s">
+        <v>45</v>
+      </c>
+      <c r="C141" t="str">
+        <f t="shared" si="6"/>
+        <v>B</v>
+      </c>
+      <c r="D141">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="B142" t="s">
+        <v>46</v>
+      </c>
+      <c r="C142" t="str">
+        <f t="shared" si="6"/>
+        <v>A</v>
+      </c>
+      <c r="D142">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="B143" t="s">
+        <v>46</v>
+      </c>
+      <c r="C143" t="str">
+        <f t="shared" si="6"/>
+        <v>A</v>
+      </c>
+      <c r="D143">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="B144" t="s">
+        <v>46</v>
+      </c>
+      <c r="C144" t="str">
+        <f t="shared" si="6"/>
+        <v>A</v>
+      </c>
+      <c r="D144">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A145">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="B145" t="s">
+        <v>46</v>
+      </c>
+      <c r="C145" t="str">
+        <f t="shared" si="6"/>
+        <v>A</v>
+      </c>
+      <c r="D145">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A146">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="B146" t="s">
+        <v>46</v>
+      </c>
+      <c r="C146" t="str">
+        <f t="shared" si="6"/>
+        <v>A</v>
+      </c>
+      <c r="D146">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A147">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="B147" t="s">
+        <v>46</v>
+      </c>
+      <c r="C147" t="str">
+        <f t="shared" si="6"/>
+        <v>A</v>
+      </c>
+      <c r="D147">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A148">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="B148" t="s">
+        <v>46</v>
+      </c>
+      <c r="C148" t="str">
+        <f t="shared" si="6"/>
+        <v>A</v>
+      </c>
+      <c r="D148">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A149">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="B149" t="s">
+        <v>46</v>
+      </c>
+      <c r="C149" t="str">
+        <f t="shared" si="6"/>
+        <v>A</v>
+      </c>
+      <c r="D149">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A150">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="B150" t="s">
+        <v>46</v>
+      </c>
+      <c r="C150" t="str">
+        <f t="shared" si="6"/>
+        <v>A</v>
+      </c>
+      <c r="D150">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="B151" t="s">
+        <v>46</v>
+      </c>
+      <c r="C151" t="str">
+        <f t="shared" si="6"/>
+        <v>A</v>
+      </c>
+      <c r="D151">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="B152" t="s">
+        <v>46</v>
+      </c>
+      <c r="C152" t="str">
+        <f t="shared" si="6"/>
+        <v>B</v>
+      </c>
+      <c r="D152">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="B153" t="s">
+        <v>46</v>
+      </c>
+      <c r="C153" t="str">
+        <f t="shared" si="6"/>
+        <v>B</v>
+      </c>
+      <c r="D153">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="B154" t="s">
+        <v>46</v>
+      </c>
+      <c r="C154" t="str">
+        <f t="shared" si="6"/>
+        <v>B</v>
+      </c>
+      <c r="D154">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="B155" t="s">
+        <v>46</v>
+      </c>
+      <c r="C155" t="str">
+        <f t="shared" si="6"/>
+        <v>B</v>
+      </c>
+      <c r="D155">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="B156" t="s">
+        <v>46</v>
+      </c>
+      <c r="C156" t="str">
+        <f t="shared" si="6"/>
+        <v>B</v>
+      </c>
+      <c r="D156">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="B157" t="s">
+        <v>46</v>
+      </c>
+      <c r="C157" t="str">
+        <f t="shared" si="6"/>
+        <v>B</v>
+      </c>
+      <c r="D157">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A158">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="B158" t="s">
+        <v>46</v>
+      </c>
+      <c r="C158" t="str">
+        <f t="shared" si="6"/>
+        <v>B</v>
+      </c>
+      <c r="D158">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A159">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="B159" t="s">
+        <v>46</v>
+      </c>
+      <c r="C159" t="str">
+        <f t="shared" si="6"/>
+        <v>B</v>
+      </c>
+      <c r="D159">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A160">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="B160" t="s">
+        <v>46</v>
+      </c>
+      <c r="C160" t="str">
+        <f t="shared" si="6"/>
+        <v>B</v>
+      </c>
+      <c r="D160">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A161">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="B161" t="s">
+        <v>46</v>
+      </c>
+      <c r="C161" t="str">
+        <f t="shared" si="6"/>
+        <v>B</v>
+      </c>
+      <c r="D161">
         <v>-1</v>
       </c>
     </row>
@@ -6187,10 +7057,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F81C51A-1511-417C-9AC3-4EF2A66959D1}">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6257,22 +7127,42 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Filled in the Rest of the Values
Filled in the rest of the values for the questionnaires.
</commit_message>
<xml_diff>
--- a/imports/vpl-fnl_pjt_data.xlsx
+++ b/imports/vpl-fnl_pjt_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roder\source\year 4 repos\HCI-FNL_PJT\imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49627DB7-A24E-483F-9154-741E73329891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF276324-C73F-49EC-AE70-1EF66FF77C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12048" yWindow="1032" windowWidth="7500" windowHeight="11112" activeTab="2" xr2:uid="{648EF0DD-0358-465E-A7D1-701403DC3CB5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{648EF0DD-0358-465E-A7D1-701403DC3CB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -1479,8 +1479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAD3DC0-0BAB-4632-81BA-A01285DC1771}">
   <dimension ref="A1:E201"/>
   <sheetViews>
-    <sheetView topLeftCell="A179" workbookViewId="0">
-      <selection activeCell="C200" sqref="C200"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="H175" sqref="H175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1521,7 +1521,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="6">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1539,7 +1539,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1557,7 +1557,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1575,7 +1575,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1702,7 +1702,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1721,7 +1721,7 @@
         <v>5</v>
       </c>
       <c r="E13" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1740,7 +1740,7 @@
         <v>5</v>
       </c>
       <c r="E14" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1759,7 +1759,7 @@
         <v>5</v>
       </c>
       <c r="E15" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1893,7 +1893,7 @@
         <v>A</v>
       </c>
       <c r="E22" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1913,7 +1913,7 @@
         <v>A</v>
       </c>
       <c r="E23" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1933,7 +1933,7 @@
         <v>A</v>
       </c>
       <c r="E24" s="9">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1953,7 +1953,7 @@
         <v>A</v>
       </c>
       <c r="E25" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -2093,7 +2093,7 @@
         <v>B</v>
       </c>
       <c r="E32" s="9">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -2113,7 +2113,7 @@
         <v>B</v>
       </c>
       <c r="E33" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -2133,7 +2133,7 @@
         <v>B</v>
       </c>
       <c r="E34" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -2153,7 +2153,7 @@
         <v>B</v>
       </c>
       <c r="E35" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -2293,7 +2293,7 @@
         <v>A</v>
       </c>
       <c r="E42" s="6">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -2313,7 +2313,7 @@
         <v>A</v>
       </c>
       <c r="E43" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -2333,7 +2333,7 @@
         <v>A</v>
       </c>
       <c r="E44" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -2353,7 +2353,7 @@
         <v>A</v>
       </c>
       <c r="E45" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -2493,7 +2493,7 @@
         <v>B</v>
       </c>
       <c r="E52" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -2513,7 +2513,7 @@
         <v>B</v>
       </c>
       <c r="E53" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -2533,7 +2533,7 @@
         <v>B</v>
       </c>
       <c r="E54" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -2553,7 +2553,7 @@
         <v>B</v>
       </c>
       <c r="E55" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -2693,7 +2693,7 @@
         <v>A</v>
       </c>
       <c r="E62" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -2713,7 +2713,7 @@
         <v>A</v>
       </c>
       <c r="E63" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -2733,7 +2733,7 @@
         <v>A</v>
       </c>
       <c r="E64" s="9">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -2753,7 +2753,7 @@
         <v>A</v>
       </c>
       <c r="E65" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -2893,7 +2893,7 @@
         <v>B</v>
       </c>
       <c r="E72" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -2913,7 +2913,7 @@
         <v>B</v>
       </c>
       <c r="E73" s="9">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
@@ -2933,7 +2933,7 @@
         <v>B</v>
       </c>
       <c r="E74" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -2953,7 +2953,7 @@
         <v>B</v>
       </c>
       <c r="E75" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
@@ -3093,7 +3093,7 @@
         <v>A</v>
       </c>
       <c r="E82" s="6">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -3113,7 +3113,7 @@
         <v>A</v>
       </c>
       <c r="E83" s="9">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -3133,7 +3133,7 @@
         <v>A</v>
       </c>
       <c r="E84" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
@@ -3153,7 +3153,7 @@
         <v>A</v>
       </c>
       <c r="E85" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -3293,7 +3293,7 @@
         <v>B</v>
       </c>
       <c r="E92" s="9">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
@@ -3313,7 +3313,7 @@
         <v>B</v>
       </c>
       <c r="E93" s="9">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
@@ -3333,7 +3333,7 @@
         <v>B</v>
       </c>
       <c r="E94" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
@@ -3353,7 +3353,7 @@
         <v>B</v>
       </c>
       <c r="E95" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
@@ -3493,7 +3493,7 @@
         <v>A</v>
       </c>
       <c r="E102" s="6">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
@@ -3513,7 +3513,7 @@
         <v>A</v>
       </c>
       <c r="E103" s="9">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
@@ -3533,7 +3533,7 @@
         <v>A</v>
       </c>
       <c r="E104" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
@@ -3553,7 +3553,7 @@
         <v>A</v>
       </c>
       <c r="E105" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
@@ -3693,7 +3693,7 @@
         <v>B</v>
       </c>
       <c r="E112" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
@@ -3713,7 +3713,7 @@
         <v>B</v>
       </c>
       <c r="E113" s="9">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
@@ -3733,7 +3733,7 @@
         <v>B</v>
       </c>
       <c r="E114" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
@@ -3753,7 +3753,7 @@
         <v>B</v>
       </c>
       <c r="E115" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
@@ -3893,7 +3893,7 @@
         <v>A</v>
       </c>
       <c r="E122" s="6">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
@@ -3913,7 +3913,7 @@
         <v>A</v>
       </c>
       <c r="E123" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
@@ -3933,7 +3933,7 @@
         <v>A</v>
       </c>
       <c r="E124" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
@@ -3953,7 +3953,7 @@
         <v>A</v>
       </c>
       <c r="E125" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
@@ -4093,7 +4093,7 @@
         <v>B</v>
       </c>
       <c r="E132" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -4113,7 +4113,7 @@
         <v>B</v>
       </c>
       <c r="E133" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -4133,7 +4133,7 @@
         <v>B</v>
       </c>
       <c r="E134" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -4153,7 +4153,7 @@
         <v>B</v>
       </c>
       <c r="E135" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
@@ -4293,7 +4293,7 @@
         <v>A</v>
       </c>
       <c r="E142" s="9">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
@@ -4313,7 +4313,7 @@
         <v>A</v>
       </c>
       <c r="E143" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
@@ -4333,7 +4333,7 @@
         <v>A</v>
       </c>
       <c r="E144" s="9">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
@@ -4353,7 +4353,7 @@
         <v>A</v>
       </c>
       <c r="E145" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
@@ -4493,7 +4493,7 @@
         <v>B</v>
       </c>
       <c r="E152" s="32">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
@@ -4513,7 +4513,7 @@
         <v>B</v>
       </c>
       <c r="E153" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
@@ -4533,7 +4533,7 @@
         <v>B</v>
       </c>
       <c r="E154" s="9">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
@@ -4553,7 +4553,7 @@
         <v>B</v>
       </c>
       <c r="E155" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
@@ -4693,7 +4693,7 @@
         <v>A</v>
       </c>
       <c r="E162" s="9">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.3">
@@ -4713,7 +4713,7 @@
         <v>A</v>
       </c>
       <c r="E163" s="9">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.3">
@@ -4733,7 +4733,7 @@
         <v>A</v>
       </c>
       <c r="E164" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.3">
@@ -4753,7 +4753,7 @@
         <v>A</v>
       </c>
       <c r="E165" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.3">
@@ -4893,7 +4893,7 @@
         <v>B</v>
       </c>
       <c r="E172" s="9">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.3">
@@ -4913,7 +4913,7 @@
         <v>B</v>
       </c>
       <c r="E173" s="9">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.3">
@@ -4933,7 +4933,7 @@
         <v>B</v>
       </c>
       <c r="E174" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
@@ -4953,7 +4953,7 @@
         <v>B</v>
       </c>
       <c r="E175" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.3">
@@ -5053,7 +5053,7 @@
         <v>B</v>
       </c>
       <c r="E180" s="9">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5093,7 +5093,7 @@
         <v>A</v>
       </c>
       <c r="E182" s="6">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.3">
@@ -5113,7 +5113,7 @@
         <v>A</v>
       </c>
       <c r="E183" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
@@ -5133,7 +5133,7 @@
         <v>A</v>
       </c>
       <c r="E184" s="9">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
@@ -5153,7 +5153,7 @@
         <v>A</v>
       </c>
       <c r="E185" s="9">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
@@ -5293,7 +5293,7 @@
         <v>B</v>
       </c>
       <c r="E192" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.3">
@@ -5313,7 +5313,7 @@
         <v>B</v>
       </c>
       <c r="E193" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.3">
@@ -5333,7 +5333,7 @@
         <v>B</v>
       </c>
       <c r="E194" s="9">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.3">
@@ -5353,7 +5353,7 @@
         <v>B</v>
       </c>
       <c r="E195" s="9">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.3">
@@ -5485,8 +5485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6155F0-D76B-402B-AB6F-C6589B98D823}">
   <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="C169" sqref="C169"/>
+    <sheetView topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="F162" sqref="F162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5527,7 +5527,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="6">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -5545,7 +5545,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -5563,7 +5563,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -5581,7 +5581,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -5708,7 +5708,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="9">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -5727,7 +5727,7 @@
         <v>5</v>
       </c>
       <c r="E13" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -5746,7 +5746,7 @@
         <v>5</v>
       </c>
       <c r="E14" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -5765,7 +5765,7 @@
         <v>5</v>
       </c>
       <c r="E15" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -5899,7 +5899,7 @@
         <v>A</v>
       </c>
       <c r="E22" s="6">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -5918,7 +5918,7 @@
         <v>A</v>
       </c>
       <c r="E23" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -5937,7 +5937,7 @@
         <v>A</v>
       </c>
       <c r="E24" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -5956,7 +5956,7 @@
         <v>A</v>
       </c>
       <c r="E25" s="9">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -6090,7 +6090,7 @@
         <v>B</v>
       </c>
       <c r="E32" s="9">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -6110,7 +6110,7 @@
         <v>B</v>
       </c>
       <c r="E33" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -6130,7 +6130,7 @@
         <v>B</v>
       </c>
       <c r="E34" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -6150,7 +6150,7 @@
         <v>B</v>
       </c>
       <c r="E35" s="9">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -6289,7 +6289,7 @@
         <v>A</v>
       </c>
       <c r="E42" s="6">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -6308,7 +6308,7 @@
         <v>A</v>
       </c>
       <c r="E43" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -6327,7 +6327,7 @@
         <v>A</v>
       </c>
       <c r="E44" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -6346,7 +6346,7 @@
         <v>A</v>
       </c>
       <c r="E45" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -6480,7 +6480,7 @@
         <v>B</v>
       </c>
       <c r="E52" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -6500,7 +6500,7 @@
         <v>B</v>
       </c>
       <c r="E53" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -6520,7 +6520,7 @@
         <v>B</v>
       </c>
       <c r="E54" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -6540,7 +6540,7 @@
         <v>B</v>
       </c>
       <c r="E55" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -6679,7 +6679,7 @@
         <v>A</v>
       </c>
       <c r="E62" s="6">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -6698,7 +6698,7 @@
         <v>A</v>
       </c>
       <c r="E63" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -6717,7 +6717,7 @@
         <v>A</v>
       </c>
       <c r="E64" s="9">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -6736,7 +6736,7 @@
         <v>A</v>
       </c>
       <c r="E65" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -6870,7 +6870,7 @@
         <v>B</v>
       </c>
       <c r="E72" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -6890,7 +6890,7 @@
         <v>B</v>
       </c>
       <c r="E73" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
@@ -6910,7 +6910,7 @@
         <v>B</v>
       </c>
       <c r="E74" s="9">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -6930,7 +6930,7 @@
         <v>B</v>
       </c>
       <c r="E75" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
@@ -7069,7 +7069,7 @@
         <v>A</v>
       </c>
       <c r="E82" s="6">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -7088,7 +7088,7 @@
         <v>A</v>
       </c>
       <c r="E83" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -7107,7 +7107,7 @@
         <v>A</v>
       </c>
       <c r="E84" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
@@ -7126,7 +7126,7 @@
         <v>A</v>
       </c>
       <c r="E85" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -7260,7 +7260,7 @@
         <v>B</v>
       </c>
       <c r="E92" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
@@ -7280,7 +7280,7 @@
         <v>B</v>
       </c>
       <c r="E93" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
@@ -7300,7 +7300,7 @@
         <v>B</v>
       </c>
       <c r="E94" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
@@ -7320,7 +7320,7 @@
         <v>B</v>
       </c>
       <c r="E95" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
@@ -7459,7 +7459,7 @@
         <v>A</v>
       </c>
       <c r="E102" s="6">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
@@ -7478,7 +7478,7 @@
         <v>A</v>
       </c>
       <c r="E103" s="9">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
@@ -7497,7 +7497,7 @@
         <v>A</v>
       </c>
       <c r="E104" s="9">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
@@ -7516,7 +7516,7 @@
         <v>A</v>
       </c>
       <c r="E105" s="9">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
@@ -7650,7 +7650,7 @@
         <v>B</v>
       </c>
       <c r="E112" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
@@ -7670,7 +7670,7 @@
         <v>B</v>
       </c>
       <c r="E113" s="9">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
@@ -7690,7 +7690,7 @@
         <v>B</v>
       </c>
       <c r="E114" s="9">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
@@ -7710,7 +7710,7 @@
         <v>B</v>
       </c>
       <c r="E115" s="9">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
@@ -7849,7 +7849,7 @@
         <v>A</v>
       </c>
       <c r="E122" s="6">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
@@ -7868,7 +7868,7 @@
         <v>A</v>
       </c>
       <c r="E123" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
@@ -7887,7 +7887,7 @@
         <v>A</v>
       </c>
       <c r="E124" s="9">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
@@ -7906,7 +7906,7 @@
         <v>A</v>
       </c>
       <c r="E125" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
@@ -8040,7 +8040,7 @@
         <v>B</v>
       </c>
       <c r="E132" s="9">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -8060,7 +8060,7 @@
         <v>B</v>
       </c>
       <c r="E133" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -8080,7 +8080,7 @@
         <v>B</v>
       </c>
       <c r="E134" s="9">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -8100,7 +8100,7 @@
         <v>B</v>
       </c>
       <c r="E135" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
@@ -8239,7 +8239,7 @@
         <v>A</v>
       </c>
       <c r="E142" s="6">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
@@ -8258,7 +8258,7 @@
         <v>A</v>
       </c>
       <c r="E143" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
@@ -8277,7 +8277,7 @@
         <v>A</v>
       </c>
       <c r="E144" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
@@ -8296,7 +8296,7 @@
         <v>A</v>
       </c>
       <c r="E145" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
@@ -8430,7 +8430,7 @@
         <v>B</v>
       </c>
       <c r="E152" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
@@ -8450,7 +8450,7 @@
         <v>B</v>
       </c>
       <c r="E153" s="9">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
@@ -8470,7 +8470,7 @@
         <v>B</v>
       </c>
       <c r="E154" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
@@ -8490,7 +8490,7 @@
         <v>B</v>
       </c>
       <c r="E155" s="9">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>